<commit_message>
Rolls back small spreadsheet to be w/o macro
Microsoft office 2013 on windows 8.1 couldn't open it
</commit_message>
<xml_diff>
--- a/src/test/resources/small-worksheet.xlsx
+++ b/src/test/resources/small-worksheet.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420" codeName="{7A2D7E96-6E34-419A-AE5F-296B3A7E7977}"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\"/>
@@ -100,70 +100,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
-          <xdr:row>23</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="CommandButton21" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,12 +364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,41 +1201,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <controls>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton21">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton21"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </controls>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
   <dimension ref="E6:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>